<commit_message>
Analysed collected data functionality added
</commit_message>
<xml_diff>
--- a/Devon_properties.xlsx
+++ b/Devon_properties.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Devon_properties" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="devon_properties" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,301 +474,301 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>No Snakes on this Plane!</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
+          <t>Rural Cabin Stunning Views</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>147</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rural Cabin Stunning Views</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+          <t>The Owl's Nest</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C4" t="n">
+        <v>143</v>
+      </c>
       <c r="D4" t="n">
-        <v>197</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Swaledale Shepherd’s Hut -in the heart of Dartmoor</t>
+          <t>A superb one bedroom apartment with sea views.</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.82</v>
+        <v>4.99</v>
       </c>
       <c r="C5" t="n">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D5" t="n">
-        <v>59</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Daffy - Meadow stay near Exeter</t>
+          <t>Countryside Cabin with Hot Tub and Tree Deck</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.82</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>356</v>
       </c>
       <c r="D6" t="n">
-        <v>68</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>The Cabin at Axe View Hideout (hot tub stay)</t>
+          <t>No Snakes on this Plane!</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.91</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>150</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
-        <v>114</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tranquil Room by the Green Field</t>
+          <t>The Cabin at Axe View Hideout (hot tub stay)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>4.91</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="D8" t="n">
-        <v>59</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Hattie - luxury secluded coastal shepherds hut</t>
+          <t>Luxury Roundhouse with log fired hot tub</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>4.97</v>
       </c>
       <c r="C9" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D9" t="n">
-        <v>71</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The Owl's Nest</t>
+          <t>Hattie - luxury secluded coastal shepherds hut</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4.99</v>
+        <v>4.97</v>
       </c>
       <c r="C10" t="n">
-        <v>143</v>
+        <v>71</v>
       </c>
       <c r="D10" t="n">
-        <v>314</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Luxury Roundhouse with log fired hot tub</t>
+          <t>'Rockpool' is a 15 minute walk to Bantham Beach.</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4.97</v>
+        <v>4.99</v>
       </c>
       <c r="C11" t="n">
-        <v>38</v>
+        <v>300</v>
       </c>
       <c r="D11" t="n">
-        <v>206</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Little Bow Green</t>
+          <t>North Devon: Treetops - Peace in Nature</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>4.95</v>
       </c>
       <c r="C12" t="n">
-        <v>274</v>
+        <v>83</v>
       </c>
       <c r="D12" t="n">
-        <v>188</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>The Wizards Cauldron -Harry Potter Themed</t>
+          <t>Tranquil Room by the Green Field</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>176</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rural Shepherds Hut Devon 25 mins from the sea</t>
+          <t>The Posh Shed</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.9</v>
+        <v>4.93</v>
       </c>
       <c r="C14" t="n">
-        <v>223</v>
+        <v>252</v>
       </c>
       <c r="D14" t="n">
-        <v>120</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Luxury Shepherds Hut with wood fired hot tub</t>
+          <t>The Shippon. Unique luxurious South Devon getaway.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>4.96</v>
       </c>
       <c r="C15" t="n">
-        <v>129</v>
+        <v>330</v>
       </c>
       <c r="D15" t="n">
-        <v>161</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Shippon. Unique luxurious South Devon getaway.</t>
+          <t>Little Owl birdhouse: Stunning sea views &amp; beach</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4.96</v>
+        <v>4.99</v>
       </c>
       <c r="C16" t="n">
-        <v>330</v>
+        <v>73</v>
       </c>
       <c r="D16" t="n">
-        <v>216</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>North Devon: Treetops - Peace in Nature</t>
+          <t>Ashmead Shepherds Hut</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4.95</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>91</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ashmead Shepherds Hut</t>
+          <t>Wolf Valley- 'The Coracle' geodesic dome ~pondside</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>5</v>
+        <v>4.95</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="D18" t="n">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Riverside Retreat- Iris the bus</t>
+          <t>Luxury Shepherds Hut with wood fired hot tub</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="D19" t="n">
-        <v>85</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cosy Cabin - Hot Tub &amp; Exmoor Views</t>
+          <t>The Lodge</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4.97</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D20" t="n">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Outstanding self-contained studio apartment</t>
+          <t>Lilypod Heron –Luxury Floating Dome Stay in Devon</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>380</v>
+        <v>30</v>
       </c>
       <c r="D21" t="n">
-        <v>117</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22">
@@ -790,477 +790,481 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Countryside Cabin with Hot Tub and Tree Deck</t>
+          <t>Cosy traditional Devon cottage</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>356</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>165</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Farm Stay Shepherds Hut, In Beautiful Oak Orchard</t>
+          <t>'The Weekender' @Cleavefarmcottages, Crackington</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>4.99</v>
       </c>
       <c r="C24" t="n">
-        <v>301</v>
+        <v>511</v>
       </c>
       <c r="D24" t="n">
-        <v>145</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Bur 2 Shepherds Hut</t>
+          <t>Cornwall Beach House - Panoramic Sea Views</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>4.89</v>
       </c>
       <c r="C25" t="n">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D25" t="n">
-        <v>147</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Haystore, Luxury Railway Carriage with Hot Tub</t>
+          <t>Glamping retreat: dome &amp; wagon with alpacas, Devon</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>4.94</v>
+        <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>625</v>
+        <v>64</v>
       </c>
       <c r="D26" t="n">
-        <v>159</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Inspiring Views &amp; Place With Free Parking By Beach</t>
+          <t>The Maple Room, Totnes, Guest Suite own entrance.</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4.86</v>
+        <v>4.91</v>
       </c>
       <c r="C27" t="n">
-        <v>152</v>
+        <v>451</v>
       </c>
       <c r="D27" t="n">
-        <v>137</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>The Shepherds Hut</t>
+          <t>Finest Retreats | Yeworthy Eco-Treehouse</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.95</v>
+        <v>4.94</v>
       </c>
       <c r="C28" t="n">
-        <v>97</v>
+        <v>390</v>
       </c>
       <c r="D28" t="n">
-        <v>94</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Unique Sea View Bungalow</t>
+          <t>Idyllic Secluded Pondside Cabin-Devon Countryside</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4.96</v>
+        <v>4.99</v>
       </c>
       <c r="C29" t="n">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="D29" t="n">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>The Nook: Tranquil Getaway with Hot Tub &amp; Sauna</t>
+          <t>Swallow View, Umberleigh, North Devon</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>4.93</v>
+        <v>4.99</v>
       </c>
       <c r="C30" t="n">
-        <v>414</v>
+        <v>281</v>
       </c>
       <c r="D30" t="n">
-        <v>174</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>"Self-contained rustic cabin with Hot Tub"</t>
+          <t>Romantic Ocean View Couples Retreat Cornwall</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>4.99</v>
       </c>
       <c r="C31" t="n">
-        <v>207</v>
+        <v>150</v>
       </c>
       <c r="D31" t="n">
-        <v>170</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Little Acorn</t>
+          <t>Cosy Shepherd's Hut in beautiful North Devon</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>4.97</v>
       </c>
       <c r="C32" t="n">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D32" t="n">
-        <v>162</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Cosy lodge, hot tub &amp; alpacas</t>
+          <t>Idyllic Shepherd Hut in Dartmoor</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>4.96</v>
       </c>
       <c r="C33" t="n">
         <v>78</v>
       </c>
       <c r="D33" t="n">
-        <v>188</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fern Hut Unique delightful space off the grid in the countryside</t>
+          <t>The Wizards Cauldron -Harry Potter Themed</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D34" t="n">
-        <v>122</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Luxury Cabin Retreat with Hot Tub - Willow</t>
+          <t>Coastal cliff top chalet, within a private garden</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>5</v>
+        <v>4.97</v>
       </c>
       <c r="C35" t="n">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="D35" t="n">
-        <v>210</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Romantic Cottage with Four-Poster Bed</t>
+          <t>The Old Stables - A Cosy Riverside Retreat</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>4.84</v>
+        <v>4.98</v>
       </c>
       <c r="C36" t="n">
-        <v>89</v>
+        <v>206</v>
       </c>
       <c r="D36" t="n">
-        <v>82</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Lilypod Heron –Luxury Floating Dome Stay in Devon</t>
+          <t>Ashridge Farm</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5</v>
+        <v>4.84</v>
       </c>
       <c r="C37" t="n">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="D37" t="n">
-        <v>258</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Modern rustic cabin near Lyme Regis</t>
+          <t>The Granary</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>4.93</v>
+        <v>4.98</v>
       </c>
       <c r="C38" t="n">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="D38" t="n">
-        <v>217</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sweetsides Shepherds Hut</t>
+          <t>Kingfisher Pod: Scenic Glamping at Milemead Lakes</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>4.96</v>
+        <v>4.93</v>
       </c>
       <c r="C39" t="n">
-        <v>119</v>
+        <v>389</v>
       </c>
       <c r="D39" t="n">
-        <v>128</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Pentlands Shepherds Hut</t>
+          <t>Fantastic coast and country retreat.</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>5</v>
+        <v>4.93</v>
       </c>
       <c r="C40" t="n">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="D40" t="n">
-        <v>138</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>“Carrabee” a beachside haven for you &amp; your pets</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
+          <t>Tranquil Shepherd's Hut with hot tub access [DWK]</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>4.91</v>
+      </c>
+      <c r="C41" t="n">
+        <v>126</v>
+      </c>
       <c r="D41" t="n">
-        <v>147</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Nestled in the Trees: A True Hideaway in Nature</t>
+          <t>Honeysuckle Shepherd Hut~Secluded ~Luxury~Hot Tub</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4.95</v>
+        <v>5</v>
       </c>
       <c r="C42" t="n">
-        <v>79</v>
+        <v>237</v>
       </c>
       <c r="D42" t="n">
-        <v>122</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Self contained apartment with beautiful gardens</t>
+          <t>Treetop cabin &amp; outdoor bath in 45 acre woodland</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4.81</v>
+        <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>160</v>
+        <v>32</v>
       </c>
       <c r="D43" t="n">
-        <v>64</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Peace, Privacy &amp; Fun !</t>
+          <t>‘The Old Laundry Room’ Unique Space</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>4.98</v>
+        <v>4.91</v>
       </c>
       <c r="C44" t="n">
-        <v>51</v>
+        <v>258</v>
       </c>
       <c r="D44" t="n">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>the pod@springwater</t>
+          <t>Cosy barn with hot tub and alpacas</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>439</v>
+        <v>59</v>
       </c>
       <c r="D45" t="n">
-        <v>208</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Coastpath Studio Retreat</t>
+          <t>Luxury Cabin Retreat with Hot Tub - Langman</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>4.91</v>
+        <v>4.99</v>
       </c>
       <c r="C46" t="n">
-        <v>101</v>
+        <v>322</v>
       </c>
       <c r="D46" t="n">
-        <v>167</v>
+        <v>203</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Modern Flat | Sea View | Coastal Path | Beach Walk</t>
+          <t>Handcrafted hut with outdoor bath</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D47" t="n">
-        <v>126</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>* NEW* Romantic rural bliss by the sea, Devon</t>
+          <t>The Drey Near Braunton NorthDevon romantic retreat</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4.98</v>
+        <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>47</v>
+        <v>261</v>
       </c>
       <c r="D48" t="n">
-        <v>140</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Willow Arch Shepherd's Hut with hot tub</t>
+          <t>The Garden Studio at the Tithe Barn</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4.98</v>
+        <v>4.8</v>
       </c>
       <c r="C49" t="n">
-        <v>197</v>
+        <v>343</v>
       </c>
       <c r="D49" t="n">
-        <v>191</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Headland Hideaway Shepherd's Hut in Lyme Regis</t>
+          <t>Shepherds hut hot tub &amp; Firepit all wood included</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4.99</v>
+        <v>4.98</v>
       </c>
       <c r="C50" t="n">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="D50" t="n">
-        <v>214</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Stylish Kingswear Coastal retreat with parking</t>
+          <t>Valley View tranquillity nr Pigs Nose</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4.95</v>
+        <v>4.98</v>
       </c>
       <c r="C51" t="n">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="D51" t="n">
-        <v>166</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>North Devon Luxury Glamping with a view!</t>
+          <t>1950's bungalow with lake views</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>4.99</v>
+        <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="D52" t="n">
-        <v>83</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>